<commit_message>
vraag gebasseerd op totale unieke vraag en aantal breng/haalmomenten foute invoer voorkomen door gegevensvalidatie toe toe voegen
</commit_message>
<xml_diff>
--- a/Python/locations_data/data_locaties.xlsx
+++ b/Python/locations_data/data_locaties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alwin\Documents\Haagse hogeschool\Modelleren\Python\locations_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julia\Documents\project 4e jaars TW\Python\locations_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44C12B-4E41-4C5A-A924-11CB8C94BCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ABBDBE-484C-4A8A-A298-FB3E85DEF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{61ED79FB-C1A9-4067-9C70-6E2BE8EE4343}"/>
+    <workbookView xWindow="375" yWindow="360" windowWidth="24960" windowHeight="14835" activeTab="1" xr2:uid="{61ED79FB-C1A9-4067-9C70-6E2BE8EE4343}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene_ziekenhuisgegevens" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="131">
   <si>
     <t>Naam</t>
   </si>
@@ -421,13 +421,16 @@
     <t>eind tijdvak ophalen</t>
   </si>
   <si>
-    <t>retour binnen (uur-uur) na begin ophaaltijdvak</t>
-  </si>
-  <si>
     <t>retour vroegst na begin ophaaltijdvak</t>
   </si>
   <si>
     <t>nee</t>
+  </si>
+  <si>
+    <t>retour binnen (uur) na begin ophaaltijdvak</t>
+  </si>
+  <si>
+    <t>Vraag_uniek_tot</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,7 +493,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -806,18 +809,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93957271-A232-4F72-9562-D274FBA7D345}">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -878,8 +881,11 @@
       <c r="T1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -940,8 +946,12 @@
       <c r="T2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <f>SUM(N2:T2)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1002,8 +1012,12 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <f t="shared" ref="U3:U55" si="0">SUM(N3:T3)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1064,8 +1078,12 @@
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1126,8 +1144,12 @@
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1188,8 +1210,12 @@
       <c r="T6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1250,8 +1276,12 @@
       <c r="T7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1312,8 +1342,12 @@
       <c r="T8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1374,8 +1408,12 @@
       <c r="T9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1436,8 +1474,12 @@
       <c r="T10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1498,8 +1540,12 @@
       <c r="T11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1560,8 +1606,12 @@
       <c r="T12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1622,8 +1672,12 @@
       <c r="T13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1684,8 +1738,12 @@
       <c r="T14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1746,8 +1804,12 @@
       <c r="T15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1808,8 +1870,12 @@
       <c r="T16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1870,8 +1936,12 @@
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1932,8 +2002,12 @@
       <c r="T18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1994,8 +2068,12 @@
       <c r="T19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U19">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2056,8 +2134,12 @@
       <c r="T20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U20">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2118,8 +2200,12 @@
       <c r="T21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2180,8 +2266,12 @@
       <c r="T22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -2242,8 +2332,12 @@
       <c r="T23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U23">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -2304,8 +2398,12 @@
       <c r="T24">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U24">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2366,8 +2464,12 @@
       <c r="T25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U25">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2428,8 +2530,12 @@
       <c r="T26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2490,8 +2596,12 @@
       <c r="T27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U27">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2552,8 +2662,12 @@
       <c r="T28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U28">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2614,8 +2728,12 @@
       <c r="T29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -2676,8 +2794,12 @@
       <c r="T30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U30">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2738,8 +2860,12 @@
       <c r="T31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U31">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -2800,8 +2926,12 @@
       <c r="T32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U32">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2862,8 +2992,12 @@
       <c r="T33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2924,8 +3058,12 @@
       <c r="T34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2986,8 +3124,12 @@
       <c r="T35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U35">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -3048,8 +3190,12 @@
       <c r="T36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U36">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -3110,8 +3256,12 @@
       <c r="T37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U37">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -3172,8 +3322,12 @@
       <c r="T38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U38">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3234,8 +3388,12 @@
       <c r="T39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U39">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -3296,8 +3454,12 @@
       <c r="T40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -3358,8 +3520,12 @@
       <c r="T41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U41">
+        <f t="shared" si="0"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -3420,8 +3586,12 @@
       <c r="T42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U42">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -3482,8 +3652,12 @@
       <c r="T43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U43">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -3544,8 +3718,12 @@
       <c r="T44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U44">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3606,8 +3784,12 @@
       <c r="T45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U45">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -3668,8 +3850,12 @@
       <c r="T46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U46">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -3730,8 +3916,12 @@
       <c r="T47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U47">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -3792,8 +3982,12 @@
       <c r="T48">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U48">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -3854,8 +4048,12 @@
       <c r="T49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U49">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -3916,8 +4114,12 @@
       <c r="T50">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -3978,8 +4180,12 @@
       <c r="T51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U51">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -4040,8 +4246,12 @@
       <c r="T52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U52">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -4102,8 +4312,12 @@
       <c r="T53">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U53">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -4164,8 +4378,12 @@
       <c r="T54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -4226,9 +4444,34 @@
       <c r="T55">
         <v>6</v>
       </c>
+      <c r="U55">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{992E0DDC-0817-46BF-AFC7-00156DA6E72B}">
+      <formula1>"bak,kar"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:T1048576" xr:uid="{344E9B99-03D6-4679-B4D5-E461EC61E196}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:T1" xr:uid="{F72FADF4-5496-4B1E-BC6F-82F4693DF115}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B524D64D-656A-4F29-A118-17281CCFEE5D}">
+          <x14:formula1>
+            <xm:f>Algemene_hubgegevens!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4236,13 +4479,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF11166C-6EB6-4481-BD27-7AC8DB248F6B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4250,7 +4493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4258,7 +4501,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4266,7 +4509,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4274,7 +4517,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -4289,24 +4532,25 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4317,10 +4561,10 @@
         <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>124</v>
@@ -4341,7 +4585,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4358,7 +4602,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="3">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
         <v>123</v>
@@ -4373,10 +4617,10 @@
         <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -4393,7 +4637,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="3">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>123</v>
@@ -4405,13 +4649,13 @@
         <v>123</v>
       </c>
       <c r="J3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -4428,7 +4672,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="3">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
         <v>123</v>
@@ -4446,7 +4690,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -4463,7 +4707,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>123</v>
@@ -4481,7 +4725,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4498,7 +4742,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>123</v>
@@ -4516,7 +4760,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -4533,7 +4777,7 @@
         <v>20.5</v>
       </c>
       <c r="F7" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
         <v>123</v>
@@ -4551,7 +4795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -4568,7 +4812,7 @@
         <v>19</v>
       </c>
       <c r="F8" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
         <v>123</v>
@@ -4586,7 +4830,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -4603,7 +4847,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>123</v>
@@ -4621,7 +4865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4638,7 +4882,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
         <v>123</v>
@@ -4656,7 +4900,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -4673,7 +4917,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="3">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
         <v>123</v>
@@ -4691,7 +4935,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -4708,7 +4952,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="3">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
         <v>123</v>
@@ -4726,7 +4970,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -4743,7 +4987,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
         <v>123</v>
@@ -4761,7 +5005,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -4778,7 +5022,7 @@
         <v>28</v>
       </c>
       <c r="F14" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
         <v>123</v>
@@ -4796,7 +5040,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -4813,7 +5057,7 @@
         <v>25</v>
       </c>
       <c r="F15" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>123</v>
@@ -4831,7 +5075,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -4848,7 +5092,7 @@
         <v>28</v>
       </c>
       <c r="F16" s="3">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
         <v>123</v>
@@ -4866,7 +5110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -4883,7 +5127,7 @@
         <v>28</v>
       </c>
       <c r="F17" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
         <v>123</v>
@@ -4901,7 +5145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -4918,7 +5162,7 @@
         <v>28</v>
       </c>
       <c r="F18" s="3">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
         <v>123</v>
@@ -4936,7 +5180,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -4953,7 +5197,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="3">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
         <v>123</v>
@@ -4971,7 +5215,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -4988,7 +5232,7 @@
         <v>25</v>
       </c>
       <c r="F20" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
         <v>123</v>
@@ -5006,7 +5250,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -5023,7 +5267,7 @@
         <v>25</v>
       </c>
       <c r="F21" s="3">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
         <v>123</v>
@@ -5041,7 +5285,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -5058,7 +5302,7 @@
         <v>24.5</v>
       </c>
       <c r="F22" s="3">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
         <v>123</v>
@@ -5076,7 +5320,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -5093,7 +5337,7 @@
         <v>24.5</v>
       </c>
       <c r="F23" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
         <v>123</v>
@@ -5111,7 +5355,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -5128,7 +5372,7 @@
         <v>24.5</v>
       </c>
       <c r="F24" s="3">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="G24" t="s">
         <v>123</v>
@@ -5146,7 +5390,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -5163,7 +5407,7 @@
         <v>24.5</v>
       </c>
       <c r="F25" s="3">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
         <v>123</v>
@@ -5181,7 +5425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -5198,7 +5442,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="3">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s">
         <v>123</v>
@@ -5216,7 +5460,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -5233,7 +5477,7 @@
         <v>24.5</v>
       </c>
       <c r="F27" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G27" t="s">
         <v>123</v>
@@ -5251,7 +5495,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -5268,7 +5512,7 @@
         <v>24.5</v>
       </c>
       <c r="F28" s="3">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
         <v>123</v>
@@ -5286,7 +5530,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -5303,7 +5547,7 @@
         <v>24.5</v>
       </c>
       <c r="F29" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G29" t="s">
         <v>123</v>
@@ -5321,7 +5565,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -5338,7 +5582,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
         <v>123</v>
@@ -5356,7 +5600,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -5373,7 +5617,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="3">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
         <v>123</v>
@@ -5391,7 +5635,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -5408,7 +5652,7 @@
         <v>30</v>
       </c>
       <c r="F32" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G32" t="s">
         <v>123</v>
@@ -5426,7 +5670,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -5443,7 +5687,7 @@
         <v>30</v>
       </c>
       <c r="F33" s="3">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="G33" t="s">
         <v>123</v>
@@ -5461,7 +5705,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -5478,7 +5722,7 @@
         <v>24.5</v>
       </c>
       <c r="F34" s="3">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
         <v>123</v>
@@ -5496,7 +5740,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -5513,7 +5757,7 @@
         <v>24.5</v>
       </c>
       <c r="F35" s="3">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="G35" t="s">
         <v>123</v>
@@ -5531,7 +5775,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -5548,7 +5792,7 @@
         <v>25</v>
       </c>
       <c r="F36" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G36" t="s">
         <v>123</v>
@@ -5566,7 +5810,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -5583,7 +5827,7 @@
         <v>28</v>
       </c>
       <c r="F37" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
         <v>123</v>
@@ -5601,7 +5845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -5618,7 +5862,7 @@
         <v>24.5</v>
       </c>
       <c r="F38" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G38" t="s">
         <v>123</v>
@@ -5636,7 +5880,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -5653,7 +5897,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G39" t="s">
         <v>123</v>
@@ -5671,7 +5915,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -5688,7 +5932,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G40" t="s">
         <v>123</v>
@@ -5706,7 +5950,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -5723,7 +5967,7 @@
         <v>14</v>
       </c>
       <c r="F41" s="3">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="G41" t="s">
         <v>123</v>
@@ -5741,7 +5985,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -5758,7 +6002,7 @@
         <v>14</v>
       </c>
       <c r="F42" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="G42" t="s">
         <v>123</v>
@@ -5776,7 +6020,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -5793,7 +6037,7 @@
         <v>14</v>
       </c>
       <c r="F43" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G43" t="s">
         <v>123</v>
@@ -5811,7 +6055,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -5828,25 +6072,25 @@
         <v>158</v>
       </c>
       <c r="F44" s="3">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="G44" t="s">
         <v>123</v>
       </c>
       <c r="H44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -5863,7 +6107,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="3">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
         <v>123</v>
@@ -5881,7 +6125,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -5898,25 +6142,25 @@
         <v>62</v>
       </c>
       <c r="F46" s="3">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="G46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K46" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -5933,25 +6177,25 @@
         <v>38</v>
       </c>
       <c r="F47" s="3">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="G47" t="s">
         <v>123</v>
       </c>
       <c r="H47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I47" t="s">
         <v>123</v>
       </c>
       <c r="J47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -5968,7 +6212,7 @@
         <v>14</v>
       </c>
       <c r="F48" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G48" t="s">
         <v>123</v>
@@ -5986,7 +6230,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -6003,25 +6247,25 @@
         <v>110</v>
       </c>
       <c r="F49" s="3">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J49" t="s">
         <v>123</v>
       </c>
       <c r="K49" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -6038,25 +6282,25 @@
         <v>38</v>
       </c>
       <c r="F50" s="3">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H50" t="s">
         <v>123</v>
       </c>
       <c r="I50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -6073,7 +6317,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="3">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G51" t="s">
         <v>123</v>
@@ -6091,7 +6335,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -6108,25 +6352,25 @@
         <v>110</v>
       </c>
       <c r="F52" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="G52" t="s">
         <v>123</v>
       </c>
       <c r="H52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K52" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -6143,25 +6387,25 @@
         <v>38</v>
       </c>
       <c r="F53" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="G53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I53" t="s">
         <v>123</v>
       </c>
       <c r="J53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K53" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -6178,25 +6422,25 @@
         <v>18</v>
       </c>
       <c r="F54" s="3">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J54" t="s">
         <v>123</v>
       </c>
       <c r="K54" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -6213,25 +6457,25 @@
         <v>42</v>
       </c>
       <c r="F55" s="3">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H55" t="s">
         <v>123</v>
       </c>
       <c r="I55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -6248,7 +6492,7 @@
         <v>24.5</v>
       </c>
       <c r="F56" s="3">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="G56" t="s">
         <v>123</v>
@@ -6267,11 +6511,33 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:K1048576" xr:uid="{F0620F03-437E-4472-BF17-D54D8BC0A4CA}">
       <formula1>"ja,nee"</formula1>
     </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C1048576" xr:uid="{40DE24A2-8D82-4EA8-9614-9B0B31E8CD93}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E1048576" xr:uid="{3C0641CC-0661-43BC-90A2-5465C27EB8A1}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{6DFA8A4C-5C8A-4A93-9C77-09BC85E0C8FE}">
+      <formula1>0</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66040660-4A9C-4574-A4F8-C99BB665A95C}">
+          <x14:formula1>
+            <xm:f>Algemene_ziekenhuisgegevens!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>